<commit_message>
working on outlier rejection
</commit_message>
<xml_diff>
--- a/GK_Data_M1.xlsx
+++ b/GK_Data_M1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cooperunion-my.sharepoint.com/personal/gabriel_kret_cooper_edu/Documents/2024-25 (Junior)/Spring 2025/ME-360-A Engineering Experimentation/M1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cooperunion-my.sharepoint.com/personal/gabriel_kret_cooper_edu/Documents/2024-25 (Junior)/Spring 2025/ME-360-A Engineering Experimentation/M1/DC-Motor-Data-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{E6123F8C-37C3-49D9-A023-A924E84BFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3661E81A-7CE7-4058-B786-B3B29DAC5A0B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{E6123F8C-37C3-49D9-A023-A924E84BFB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3825E47C-98A9-4898-9BD2-8C3EA560F99D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-225" windowWidth="29040" windowHeight="15720" xr2:uid="{8958E2FF-0A7F-4C14-A595-290FA2A44AE1}"/>
+    <workbookView minimized="1" xWindow="4755" yWindow="1890" windowWidth="21600" windowHeight="12450" xr2:uid="{8958E2FF-0A7F-4C14-A595-290FA2A44AE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -531,28 +531,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25D5201-816A-48C5-95E8-0E58B856CDCF}">
   <dimension ref="A1:O155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A155"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -596,7 +596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -663,7 +663,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -695,7 +695,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -727,7 +727,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -791,7 +791,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -823,7 +823,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -855,7 +855,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -887,7 +887,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -919,7 +919,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1015,7 +1015,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1079,7 +1079,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1111,7 +1111,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1143,7 +1143,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1239,7 +1239,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1338,7 +1338,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1370,7 +1370,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -1530,7 +1530,7 @@
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -1562,7 +1562,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -1594,7 +1594,7 @@
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -1626,7 +1626,7 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -1754,7 +1754,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -1786,7 +1786,7 @@
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -1818,7 +1818,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -1850,7 +1850,7 @@
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1981,7 +1981,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2013,7 +2013,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2045,7 +2045,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2077,7 +2077,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2109,7 +2109,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2141,7 +2141,7 @@
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2173,7 +2173,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2205,7 +2205,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2237,7 +2237,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2333,7 +2333,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2429,7 +2429,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2493,7 +2493,7 @@
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2525,7 +2525,7 @@
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2720,7 +2720,7 @@
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -2816,7 +2816,7 @@
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -2880,7 +2880,7 @@
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -2912,7 +2912,7 @@
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -2976,7 +2976,7 @@
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -3008,7 +3008,7 @@
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -3072,7 +3072,7 @@
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -3139,7 +3139,7 @@
       <c r="M80" s="7"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -3171,7 +3171,7 @@
       <c r="M81" s="7"/>
       <c r="N81" s="7"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -3203,7 +3203,7 @@
       <c r="M82" s="7"/>
       <c r="N82" s="7"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -3235,7 +3235,7 @@
       <c r="M83" s="7"/>
       <c r="N83" s="7"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="M84" s="7"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -3299,7 +3299,7 @@
       <c r="M85" s="7"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="M86" s="7"/>
       <c r="N86" s="7"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="M87" s="7"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -3395,7 +3395,7 @@
       <c r="M88" s="7"/>
       <c r="N88" s="7"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>88</v>
       </c>
@@ -3427,7 +3427,7 @@
       <c r="M89" s="7"/>
       <c r="N89" s="7"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="M90" s="7"/>
       <c r="N90" s="7"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -3491,7 +3491,7 @@
       <c r="M91" s="7"/>
       <c r="N91" s="7"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -3523,7 +3523,7 @@
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -3555,7 +3555,7 @@
       <c r="M93" s="7"/>
       <c r="N93" s="7"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="M94" s="7"/>
       <c r="N94" s="7"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -3619,7 +3619,7 @@
       <c r="M95" s="7"/>
       <c r="N95" s="7"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -3651,7 +3651,7 @@
       <c r="M96" s="7"/>
       <c r="N96" s="7"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="M97" s="7"/>
       <c r="N97" s="7"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -3715,7 +3715,7 @@
       <c r="M98" s="7"/>
       <c r="N98" s="7"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -3782,7 +3782,7 @@
       <c r="M100" s="5"/>
       <c r="N100" s="5"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -3814,7 +3814,7 @@
       <c r="M101" s="5"/>
       <c r="N101" s="5"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -3846,12 +3846,12 @@
       <c r="M102" s="5"/>
       <c r="N102" s="5"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <v>102</v>
       </c>
       <c r="B103" s="5">
-        <v>283</v>
+        <v>183</v>
       </c>
       <c r="C103" s="5">
         <v>65</v>
@@ -3878,7 +3878,7 @@
       <c r="M103" s="5"/>
       <c r="N103" s="5"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="M104" s="5"/>
       <c r="N104" s="5"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="M105" s="5"/>
       <c r="N105" s="5"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -3974,7 +3974,7 @@
       <c r="M106" s="5"/>
       <c r="N106" s="5"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -4006,7 +4006,7 @@
       <c r="M107" s="5"/>
       <c r="N107" s="5"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -4038,7 +4038,7 @@
       <c r="M108" s="5"/>
       <c r="N108" s="5"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="M109" s="5"/>
       <c r="N109" s="5"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -4102,7 +4102,7 @@
       <c r="M110" s="5"/>
       <c r="N110" s="5"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -4134,7 +4134,7 @@
       <c r="M111" s="5"/>
       <c r="N111" s="5"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="M112" s="5"/>
       <c r="N112" s="5"/>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -4198,7 +4198,7 @@
       <c r="M113" s="5"/>
       <c r="N113" s="5"/>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -4230,7 +4230,7 @@
       <c r="M114" s="5"/>
       <c r="N114" s="5"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -4262,7 +4262,7 @@
       <c r="M115" s="5"/>
       <c r="N115" s="5"/>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -4294,7 +4294,7 @@
       <c r="M116" s="5"/>
       <c r="N116" s="5"/>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -4326,7 +4326,7 @@
       <c r="M117" s="5"/>
       <c r="N117" s="5"/>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -4358,7 +4358,7 @@
       <c r="M118" s="5"/>
       <c r="N118" s="5"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -4425,7 +4425,7 @@
       <c r="M120" s="4"/>
       <c r="N120" s="4"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -4457,7 +4457,7 @@
       <c r="M121" s="4"/>
       <c r="N121" s="4"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="M122" s="4"/>
       <c r="N122" s="4"/>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -4521,7 +4521,7 @@
       <c r="M123" s="4"/>
       <c r="N123" s="4"/>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -4553,7 +4553,7 @@
       <c r="M124" s="4"/>
       <c r="N124" s="4"/>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -4585,7 +4585,7 @@
       <c r="M125" s="4"/>
       <c r="N125" s="4"/>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -4617,7 +4617,7 @@
       <c r="M126" s="4"/>
       <c r="N126" s="4"/>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -4649,7 +4649,7 @@
       <c r="M127" s="4"/>
       <c r="N127" s="4"/>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -4681,7 +4681,7 @@
       <c r="M128" s="4"/>
       <c r="N128" s="4"/>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -4713,7 +4713,7 @@
       <c r="M129" s="4"/>
       <c r="N129" s="4"/>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -4745,7 +4745,7 @@
       <c r="M130" s="4"/>
       <c r="N130" s="4"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -4777,7 +4777,7 @@
       <c r="M131" s="4"/>
       <c r="N131" s="4"/>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -4809,7 +4809,7 @@
       <c r="M132" s="4"/>
       <c r="N132" s="4"/>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -4841,7 +4841,7 @@
       <c r="M133" s="4"/>
       <c r="N133" s="4"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -4873,7 +4873,7 @@
       <c r="M134" s="4"/>
       <c r="N134" s="4"/>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -4905,7 +4905,7 @@
       <c r="M135" s="4"/>
       <c r="N135" s="4"/>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <v>135</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="8">
         <v>136</v>
       </c>
@@ -4973,7 +4973,7 @@
       <c r="M137" s="8"/>
       <c r="N137" s="8"/>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <v>137</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="M138" s="8"/>
       <c r="N138" s="8"/>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>138</v>
       </c>
@@ -5038,7 +5038,7 @@
       <c r="M139" s="8"/>
       <c r="N139" s="8"/>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <v>139</v>
       </c>
@@ -5071,7 +5071,7 @@
       <c r="M140" s="8"/>
       <c r="N140" s="8"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>140</v>
       </c>
@@ -5104,7 +5104,7 @@
       <c r="M141" s="8"/>
       <c r="N141" s="8"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <v>141</v>
       </c>
@@ -5136,7 +5136,7 @@
       <c r="M142" s="8"/>
       <c r="N142" s="8"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>142</v>
       </c>
@@ -5169,7 +5169,7 @@
       <c r="M143" s="8"/>
       <c r="N143" s="8"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <v>143</v>
       </c>
@@ -5202,7 +5202,7 @@
       <c r="M144" s="8"/>
       <c r="N144" s="8"/>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>144</v>
       </c>
@@ -5235,7 +5235,7 @@
       <c r="M145" s="8"/>
       <c r="N145" s="8"/>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>145</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="M146" s="8"/>
       <c r="N146" s="8"/>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>146</v>
       </c>
@@ -5301,7 +5301,7 @@
       <c r="M147" s="8"/>
       <c r="N147" s="8"/>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>147</v>
       </c>
@@ -5334,7 +5334,7 @@
       <c r="M148" s="8"/>
       <c r="N148" s="8"/>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <v>148</v>
       </c>
@@ -5367,7 +5367,7 @@
       <c r="M149" s="8"/>
       <c r="N149" s="8"/>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="8">
         <v>149</v>
       </c>
@@ -5400,7 +5400,7 @@
       <c r="M150" s="8"/>
       <c r="N150" s="8"/>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="8">
         <v>150</v>
       </c>
@@ -5433,7 +5433,7 @@
       <c r="M151" s="8"/>
       <c r="N151" s="8"/>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <v>151</v>
       </c>
@@ -5466,7 +5466,7 @@
       <c r="M152" s="8"/>
       <c r="N152" s="8"/>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" s="8">
         <v>152</v>
       </c>
@@ -5499,7 +5499,7 @@
       <c r="M153" s="8"/>
       <c r="N153" s="8"/>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" s="8">
         <v>153</v>
       </c>
@@ -5532,7 +5532,7 @@
       <c r="M154" s="8"/>
       <c r="N154" s="8"/>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" s="8">
         <v>154</v>
       </c>

</xml_diff>